<commit_message>
fixed model != database
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF/forms/MIF/MIF.xlsx
+++ b/app/config/tables/MIF/forms/MIF/MIF.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15115E0F-E2AA-4B2C-9503-79D9DD174541}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C019F5-C819-47DB-BA9C-F328D88652E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="648" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="648" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -6957,8 +6957,8 @@
   <dimension ref="A1:G313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D310" sqref="D310"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7568,7 +7568,7 @@
         <v>383</v>
       </c>
       <c r="B56" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -10814,7 +10814,7 @@
   <dimension ref="A1:R140"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -12186,8 +12186,8 @@
   <dimension ref="A1:XFD117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix in MIF + deleted not usefill files
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF/forms/MIF/MIF.xlsx
+++ b/app/config/tables/MIF/forms/MIF/MIF.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C019F5-C819-47DB-BA9C-F328D88652E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4DDAB4-0AF9-410F-AD0E-2D86AA4E0BF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="648" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="648" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -3851,7 +3851,7 @@
     <t>Last visit status: &lt;b&gt;Não visitada&lt;b&gt;</t>
   </si>
   <si>
-    <t>data('ESTADOVIS') != '2' &amp;&amp; data('ESTADOVIS') !='3' &amp;&amp; data('ESTADOVIS') == '6'</t>
+    <t>data('ESTADOVIS') != '2' &amp;&amp; data('ESTADOVIS') !='3'</t>
   </si>
 </sst>
 </file>
@@ -4619,8 +4619,8 @@
   <dimension ref="A1:D156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77:A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6956,7 +6956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:G313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
     </sheetView>
@@ -12185,9 +12185,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568D4494-839B-4F7A-8E9C-72B7EC0E8A88}">
   <dimension ref="A1:XFD117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added "today" function to adate
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF/forms/MIF/MIF.xlsx
+++ b/app/config/tables/MIF/forms/MIF/MIF.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFE8DBD-8BAC-4F1E-AD6D-5AAEA47BC22D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3BBEB6-1B64-44E5-8553-24C0A22C2058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="649" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="649" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -4231,7 +4231,7 @@
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11365,9 +11365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568D4494-839B-4F7A-8E9C-72B7EC0E8A88}">
   <dimension ref="A1:N146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E94" sqref="E94"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12930,9 +12930,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF620B59-79FA-4646-92DD-ED95E169989F}">
   <dimension ref="A1:M481"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13143,7 +13143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="29" t="s">
         <v>113</v>
       </c>
@@ -17981,6 +17981,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>